<commit_message>
modified properties file and changed url
</commit_message>
<xml_diff>
--- a/rafiMavenStock/TestInputs/InputSheet.xlsx
+++ b/rafiMavenStock/TestInputs/InputSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1155" windowWidth="13980" windowHeight="8025"/>
+    <workbookView xWindow="0" yWindow="2430" windowWidth="10680" windowHeight="3390"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestCases" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,8 @@
     <sheet name="SupplierCreation" sheetId="3" r:id="rId3"/>
     <sheet name="StockCategories" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:I10"/>
 </workbook>
 </file>
 
@@ -388,8 +389,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,6 +478,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -555,6 +561,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -589,6 +596,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -764,20 +772,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -791,7 +799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -802,7 +810,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -813,7 +821,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -830,23 +838,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -866,7 +874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -883,7 +891,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -900,7 +908,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -917,7 +925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -934,7 +942,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -951,7 +959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -968,7 +976,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -985,7 +993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1002,7 +1010,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1019,7 +1027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1036,7 +1044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1053,7 +1061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1070,7 +1078,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1093,23 +1101,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="21">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1129,7 +1137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -1147,7 +1155,7 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1165,7 +1173,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1183,7 +1191,7 @@
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -1201,7 +1209,7 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -1219,7 +1227,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1237,7 +1245,7 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -1255,7 +1263,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -1273,7 +1281,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -1291,7 +1299,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
@@ -1309,7 +1317,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
@@ -1327,7 +1335,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A13" s="4" t="s">
         <v>47</v>
       </c>
@@ -1345,7 +1353,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A14" s="4" t="s">
         <v>91</v>
       </c>
@@ -1363,7 +1371,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A15" s="4" t="s">
         <v>48</v>
       </c>
@@ -1381,7 +1389,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A16" s="4" t="s">
         <v>120</v>
       </c>
@@ -1399,7 +1407,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="17" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A17" s="4" t="s">
         <v>50</v>
       </c>
@@ -1417,7 +1425,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="18" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A18" s="4" t="s">
         <v>52</v>
       </c>
@@ -1435,7 +1443,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="19" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A19" s="4" t="s">
         <v>54</v>
       </c>
@@ -1453,7 +1461,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="20" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
@@ -1471,7 +1479,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="21" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A21" s="4" t="s">
         <v>58</v>
       </c>
@@ -1489,7 +1497,7 @@
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="22" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A22" s="4" t="s">
         <v>60</v>
       </c>
@@ -1507,7 +1515,7 @@
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="23" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A23" s="4" t="s">
         <v>62</v>
       </c>
@@ -1525,7 +1533,7 @@
       </c>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="24" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A24" s="4" t="s">
         <v>64</v>
       </c>
@@ -1543,7 +1551,7 @@
       </c>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="25" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A25" s="4" t="s">
         <v>67</v>
       </c>
@@ -1561,7 +1569,7 @@
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="26" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A26" s="4" t="s">
         <v>68</v>
       </c>
@@ -1579,7 +1587,7 @@
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="27" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A27" s="4" t="s">
         <v>70</v>
       </c>
@@ -1597,7 +1605,7 @@
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="28" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A28" s="4" t="s">
         <v>71</v>
       </c>
@@ -1615,7 +1623,7 @@
       </c>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="29" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A29" s="4" t="s">
         <v>73</v>
       </c>
@@ -1633,7 +1641,7 @@
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="30" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A30" s="4" t="s">
         <v>75</v>
       </c>
@@ -1651,7 +1659,7 @@
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="31" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A31" s="4" t="s">
         <v>77</v>
       </c>
@@ -1669,7 +1677,7 @@
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="32" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A32" s="4" t="s">
         <v>78</v>
       </c>
@@ -1687,7 +1695,7 @@
       </c>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="33" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A33" s="4" t="s">
         <v>80</v>
       </c>
@@ -1705,7 +1713,7 @@
       </c>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="34" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A34" s="4" t="s">
         <v>118</v>
       </c>
@@ -1723,7 +1731,7 @@
       </c>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="35" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A35" s="4" t="s">
         <v>45</v>
       </c>
@@ -1741,7 +1749,7 @@
       </c>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="36" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A36" s="4" t="s">
         <v>84</v>
       </c>
@@ -1759,7 +1767,7 @@
       </c>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="37" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A37" s="4" t="s">
         <v>85</v>
       </c>
@@ -1777,7 +1785,7 @@
       </c>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="38" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A38" s="4" t="s">
         <v>87</v>
       </c>
@@ -1795,7 +1803,7 @@
       </c>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="39" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A39" s="4" t="s">
         <v>88</v>
       </c>
@@ -1813,7 +1821,7 @@
       </c>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="40" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A40" s="4" t="s">
         <v>90</v>
       </c>
@@ -1831,7 +1839,7 @@
       </c>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="18.75">
+    <row r="41" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
         <v>95</v>
       </c>
@@ -1859,23 +1867,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="21">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1895,7 +1903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1912,7 +1920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1929,7 +1937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1946,7 +1954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1963,7 +1971,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1980,7 +1988,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1997,7 +2005,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>97</v>
       </c>
@@ -2014,7 +2022,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>98</v>
       </c>
@@ -2031,7 +2039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>100</v>
       </c>
@@ -2048,7 +2056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
@@ -2065,7 +2073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>84</v>
       </c>
@@ -2082,7 +2090,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>103</v>
       </c>
@@ -2099,7 +2107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>105</v>
       </c>
@@ -2116,7 +2124,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
@@ -2133,7 +2141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="21">
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>108</v>
       </c>
@@ -2150,7 +2158,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" ht="21">
+    <row r="17" spans="1:5" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>109</v>
       </c>
@@ -2167,7 +2175,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" ht="21">
+    <row r="18" spans="1:5" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>110</v>
       </c>
@@ -2184,7 +2192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="1" customFormat="1" ht="21">
+    <row r="19" spans="1:5" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>111</v>
       </c>
@@ -2201,7 +2209,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" ht="21">
+    <row r="20" spans="1:5" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>112</v>
       </c>
@@ -2218,7 +2226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" ht="21">
+    <row r="21" spans="1:5" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>95</v>
       </c>

</xml_diff>